<commit_message>
"#1 added ability to process multiple sheets/tabs. Renamed IX class. Sheet class supercedes Header class. Added more formating for clarity.
</commit_message>
<xml_diff>
--- a/input_files/afcrs/CA_Clayton_2022.xlsx
+++ b/input_files/afcrs/CA_Clayton_2022.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10910"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Aug05\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katrinawheelan/Desktop/Code/CLOSUP/process_xbrl/process-xbrl/input_files/afcrs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B51AE399-1497-4B33-BD11-DBDC67685C0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B175915-7FF3-0C46-BAF2-D37992959F09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1080" windowWidth="25200" windowHeight="14355" tabRatio="834" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1960" yWindow="1080" windowWidth="25200" windowHeight="14360" tabRatio="834" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Statement of Net Position" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="745" uniqueCount="363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="745" uniqueCount="362">
   <si>
     <t>City of Clayton</t>
   </si>
@@ -57,9 +57,6 @@
   </si>
   <si>
     <t>Governmental Activities</t>
-  </si>
-  <si>
-    <t>Business-Type Activites</t>
   </si>
   <si>
     <t>Total</t>
@@ -1288,7 +1285,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
@@ -1417,7 +1414,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1725,18 +1721,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="44.42578125" customWidth="1"/>
-    <col min="2" max="2" width="41.5703125" customWidth="1"/>
-    <col min="3" max="5" width="18.7109375" customWidth="1"/>
+    <col min="1" max="1" width="44.5" customWidth="1"/>
+    <col min="2" max="2" width="41.5" customWidth="1"/>
+    <col min="3" max="5" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75">
+    <row r="1" spans="1:5" ht="16">
       <c r="A1" s="17"/>
       <c r="B1" s="54" t="s">
         <v>0</v>
@@ -1745,7 +1741,7 @@
       <c r="D1" s="55"/>
       <c r="E1" s="55"/>
     </row>
-    <row r="2" spans="1:5" ht="15.75">
+    <row r="2" spans="1:5" ht="16">
       <c r="A2" s="17"/>
       <c r="B2" s="54" t="s">
         <v>1</v>
@@ -1754,7 +1750,7 @@
       <c r="D2" s="55"/>
       <c r="E2" s="55"/>
     </row>
-    <row r="3" spans="1:5" ht="15.75">
+    <row r="3" spans="1:5" ht="16">
       <c r="A3" s="17"/>
       <c r="B3" s="54" t="s">
         <v>2</v>
@@ -1763,7 +1759,7 @@
       <c r="D3" s="55"/>
       <c r="E3" s="55"/>
     </row>
-    <row r="4" spans="1:5" ht="15.75">
+    <row r="4" spans="1:5" ht="16">
       <c r="A4" s="17"/>
       <c r="B4" s="54" t="s">
         <v>3</v>
@@ -1772,7 +1768,7 @@
       <c r="D4" s="55"/>
       <c r="E4" s="55"/>
     </row>
-    <row r="5" spans="1:5" ht="30">
+    <row r="5" spans="1:5" ht="32">
       <c r="A5" s="20" t="s">
         <v>4</v>
       </c>
@@ -1781,16 +1777,16 @@
         <v>5</v>
       </c>
       <c r="D5" s="57" t="s">
+        <v>125</v>
+      </c>
+      <c r="E5" s="57" t="s">
         <v>6</v>
-      </c>
-      <c r="E5" s="57" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15">
       <c r="A6" s="20"/>
       <c r="B6" s="56" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" s="58"/>
       <c r="D6" s="58"/>
@@ -1799,7 +1795,7 @@
     <row r="7" spans="1:5" ht="15">
       <c r="A7" s="20"/>
       <c r="B7" s="56" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" s="56"/>
       <c r="D7" s="56"/>
@@ -1807,16 +1803,16 @@
     </row>
     <row r="8" spans="1:5" ht="15">
       <c r="A8" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="56" t="s">
         <v>10</v>
-      </c>
-      <c r="B8" s="56" t="s">
-        <v>11</v>
       </c>
       <c r="C8" s="59">
         <v>13441679</v>
       </c>
       <c r="D8" s="58" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E8" s="59">
         <v>13441679</v>
@@ -1824,16 +1820,16 @@
     </row>
     <row r="9" spans="1:5" ht="15">
       <c r="A9" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="56" t="s">
         <v>13</v>
-      </c>
-      <c r="B9" s="56" t="s">
-        <v>14</v>
       </c>
       <c r="C9" s="60">
         <v>1133315</v>
       </c>
       <c r="D9" s="58" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E9" s="60">
         <v>1133315</v>
@@ -1841,16 +1837,16 @@
     </row>
     <row r="10" spans="1:5" ht="15">
       <c r="A10" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="56" t="s">
         <v>16</v>
-      </c>
-      <c r="B10" s="56" t="s">
-        <v>17</v>
       </c>
       <c r="C10" s="60">
         <v>25257</v>
       </c>
       <c r="D10" s="58" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E10" s="60">
         <v>25257</v>
@@ -1858,10 +1854,10 @@
     </row>
     <row r="11" spans="1:5" ht="15">
       <c r="A11" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="56" t="s">
         <v>18</v>
-      </c>
-      <c r="B11" s="56" t="s">
-        <v>19</v>
       </c>
       <c r="C11" s="60">
         <v>120893</v>
@@ -1870,21 +1866,21 @@
         <v>-120893</v>
       </c>
       <c r="E11" s="58" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15">
       <c r="A12" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="56" t="s">
         <v>20</v>
-      </c>
-      <c r="B12" s="56" t="s">
-        <v>21</v>
       </c>
       <c r="C12" s="60">
         <v>52578</v>
       </c>
       <c r="D12" s="58" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E12" s="60">
         <v>52578</v>
@@ -1892,10 +1888,10 @@
     </row>
     <row r="13" spans="1:5" ht="15">
       <c r="A13" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="56" t="s">
         <v>22</v>
-      </c>
-      <c r="B13" s="56" t="s">
-        <v>23</v>
       </c>
       <c r="C13" s="60">
         <v>14773722</v>
@@ -1910,7 +1906,7 @@
     <row r="14" spans="1:5" ht="15">
       <c r="A14" s="20"/>
       <c r="B14" s="56" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C14" s="56"/>
       <c r="D14" s="56"/>
@@ -1918,16 +1914,16 @@
     </row>
     <row r="15" spans="1:5" ht="15">
       <c r="A15" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="56" t="s">
         <v>25</v>
-      </c>
-      <c r="B15" s="56" t="s">
-        <v>26</v>
       </c>
       <c r="C15" s="60">
         <v>3170453</v>
       </c>
       <c r="D15" s="58" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E15" s="60">
         <v>3170453</v>
@@ -1935,16 +1931,16 @@
     </row>
     <row r="16" spans="1:5" ht="15">
       <c r="A16" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="56" t="s">
         <v>27</v>
-      </c>
-      <c r="B16" s="56" t="s">
-        <v>28</v>
       </c>
       <c r="C16" s="60">
         <v>3311550</v>
       </c>
       <c r="D16" s="58" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E16" s="60">
         <v>3311550</v>
@@ -1952,10 +1948,10 @@
     </row>
     <row r="17" spans="1:5" ht="15">
       <c r="A17" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="56" t="s">
         <v>29</v>
-      </c>
-      <c r="B17" s="56" t="s">
-        <v>30</v>
       </c>
       <c r="C17" s="60">
         <v>3133754</v>
@@ -1969,10 +1965,10 @@
     </row>
     <row r="18" spans="1:5" ht="15">
       <c r="A18" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="56" t="s">
         <v>31</v>
-      </c>
-      <c r="B18" s="56" t="s">
-        <v>32</v>
       </c>
       <c r="C18" s="60">
         <v>25982451</v>
@@ -1986,10 +1982,10 @@
     </row>
     <row r="19" spans="1:5" ht="15">
       <c r="A19" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="56" t="s">
         <v>33</v>
-      </c>
-      <c r="B19" s="56" t="s">
-        <v>34</v>
       </c>
       <c r="C19" s="60">
         <v>35598208</v>
@@ -2003,10 +1999,10 @@
     </row>
     <row r="20" spans="1:5" ht="15">
       <c r="A20" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="56" t="s">
         <v>35</v>
-      </c>
-      <c r="B20" s="56" t="s">
-        <v>36</v>
       </c>
       <c r="C20" s="61">
         <v>50371930</v>
@@ -2028,7 +2024,7 @@
     <row r="22" spans="1:5" ht="15">
       <c r="A22" s="20"/>
       <c r="B22" s="56" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C22" s="56"/>
       <c r="D22" s="56"/>
@@ -2036,16 +2032,16 @@
     </row>
     <row r="23" spans="1:5" ht="15">
       <c r="A23" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="B23" s="56" t="s">
         <v>38</v>
-      </c>
-      <c r="B23" s="56" t="s">
-        <v>39</v>
       </c>
       <c r="C23" s="60">
         <v>1285641</v>
       </c>
       <c r="D23" s="58" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E23" s="60">
         <v>1285641</v>
@@ -2053,33 +2049,33 @@
     </row>
     <row r="24" spans="1:5" ht="15">
       <c r="A24" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" s="56" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="56" t="s">
-        <v>41</v>
-      </c>
       <c r="C24" s="58" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D24" s="58" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E24" s="58" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="15">
       <c r="A25" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25" s="56" t="s">
         <v>42</v>
-      </c>
-      <c r="B25" s="56" t="s">
-        <v>43</v>
       </c>
       <c r="C25" s="61">
         <v>1285641</v>
       </c>
       <c r="D25" s="62" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E25" s="61">
         <v>1285641</v>
@@ -2095,7 +2091,7 @@
     <row r="27" spans="1:5" ht="15">
       <c r="A27" s="20"/>
       <c r="B27" s="56" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C27" s="56"/>
       <c r="D27" s="56"/>
@@ -2104,7 +2100,7 @@
     <row r="28" spans="1:5" ht="15">
       <c r="A28" s="20"/>
       <c r="B28" s="56" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C28" s="56"/>
       <c r="D28" s="56"/>
@@ -2112,10 +2108,10 @@
     </row>
     <row r="29" spans="1:5" ht="15">
       <c r="A29" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="B29" s="56" t="s">
         <v>46</v>
-      </c>
-      <c r="B29" s="56" t="s">
-        <v>47</v>
       </c>
       <c r="C29" s="60">
         <v>149907</v>
@@ -2129,13 +2125,13 @@
     </row>
     <row r="30" spans="1:5" ht="15">
       <c r="A30" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="B30" s="56" t="s">
         <v>48</v>
       </c>
-      <c r="B30" s="56" t="s">
-        <v>49</v>
-      </c>
       <c r="C30" s="58" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D30" s="60">
         <v>5500</v>
@@ -2146,16 +2142,16 @@
     </row>
     <row r="31" spans="1:5" ht="15">
       <c r="A31" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="B31" s="56" t="s">
         <v>50</v>
-      </c>
-      <c r="B31" s="56" t="s">
-        <v>51</v>
       </c>
       <c r="C31" s="63">
         <v>37</v>
       </c>
       <c r="D31" s="58" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E31" s="63">
         <v>37</v>
@@ -2163,16 +2159,16 @@
     </row>
     <row r="32" spans="1:5" ht="15">
       <c r="A32" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="B32" s="56" t="s">
         <v>52</v>
-      </c>
-      <c r="B32" s="56" t="s">
-        <v>53</v>
       </c>
       <c r="C32" s="60">
         <v>332166</v>
       </c>
       <c r="D32" s="58" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E32" s="60">
         <v>332166</v>
@@ -2180,16 +2176,16 @@
     </row>
     <row r="33" spans="1:5" ht="15">
       <c r="A33" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="B33" s="56" t="s">
         <v>54</v>
-      </c>
-      <c r="B33" s="56" t="s">
-        <v>55</v>
       </c>
       <c r="C33" s="60">
         <v>83645</v>
       </c>
       <c r="D33" s="58" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E33" s="60">
         <v>83645</v>
@@ -2197,16 +2193,16 @@
     </row>
     <row r="34" spans="1:5" ht="15">
       <c r="A34" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="B34" s="56" t="s">
         <v>56</v>
-      </c>
-      <c r="B34" s="56" t="s">
-        <v>57</v>
       </c>
       <c r="C34" s="60">
         <v>74358</v>
       </c>
       <c r="D34" s="58" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E34" s="60">
         <v>74358</v>
@@ -2214,10 +2210,10 @@
     </row>
     <row r="35" spans="1:5" ht="15">
       <c r="A35" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B35" s="56" t="s">
         <v>58</v>
-      </c>
-      <c r="B35" s="56" t="s">
-        <v>59</v>
       </c>
       <c r="C35" s="60">
         <v>640113</v>
@@ -2232,7 +2228,7 @@
     <row r="36" spans="1:5" ht="15">
       <c r="A36" s="20"/>
       <c r="B36" s="56" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C36" s="56"/>
       <c r="D36" s="56"/>
@@ -2240,16 +2236,16 @@
     </row>
     <row r="37" spans="1:5" ht="15">
       <c r="A37" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="B37" s="56" t="s">
         <v>61</v>
-      </c>
-      <c r="B37" s="56" t="s">
-        <v>62</v>
       </c>
       <c r="C37" s="60">
         <v>83645</v>
       </c>
       <c r="D37" s="58" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E37" s="60">
         <v>83645</v>
@@ -2257,16 +2253,16 @@
     </row>
     <row r="38" spans="1:5" ht="15">
       <c r="A38" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="B38" s="56" t="s">
         <v>63</v>
-      </c>
-      <c r="B38" s="56" t="s">
-        <v>64</v>
       </c>
       <c r="C38" s="60">
         <v>578315</v>
       </c>
       <c r="D38" s="58" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E38" s="60">
         <v>578315</v>
@@ -2274,16 +2270,16 @@
     </row>
     <row r="39" spans="1:5" ht="15">
       <c r="A39" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="B39" s="56" t="s">
         <v>65</v>
-      </c>
-      <c r="B39" s="56" t="s">
-        <v>66</v>
       </c>
       <c r="C39" s="60">
         <v>2759739</v>
       </c>
       <c r="D39" s="58" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E39" s="60">
         <v>2759739</v>
@@ -2291,16 +2287,16 @@
     </row>
     <row r="40" spans="1:5" ht="15">
       <c r="A40" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="B40" s="56" t="s">
         <v>67</v>
-      </c>
-      <c r="B40" s="56" t="s">
-        <v>68</v>
       </c>
       <c r="C40" s="60">
         <v>244640</v>
       </c>
       <c r="D40" s="58" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E40" s="60">
         <v>244640</v>
@@ -2308,16 +2304,16 @@
     </row>
     <row r="41" spans="1:5" ht="15">
       <c r="A41" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="B41" s="56" t="s">
         <v>69</v>
-      </c>
-      <c r="B41" s="56" t="s">
-        <v>70</v>
       </c>
       <c r="C41" s="60">
         <v>3666339</v>
       </c>
       <c r="D41" s="58" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E41" s="60">
         <v>3666339</v>
@@ -2325,10 +2321,10 @@
     </row>
     <row r="42" spans="1:5" ht="15">
       <c r="A42" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="B42" s="56" t="s">
         <v>71</v>
-      </c>
-      <c r="B42" s="56" t="s">
-        <v>72</v>
       </c>
       <c r="C42" s="61">
         <v>4306452</v>
@@ -2350,7 +2346,7 @@
     <row r="44" spans="1:5" ht="15">
       <c r="A44" s="20"/>
       <c r="B44" s="56" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C44" s="56"/>
       <c r="D44" s="56"/>
@@ -2358,16 +2354,16 @@
     </row>
     <row r="45" spans="1:5" ht="15">
       <c r="A45" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="B45" s="56" t="s">
         <v>74</v>
-      </c>
-      <c r="B45" s="56" t="s">
-        <v>75</v>
       </c>
       <c r="C45" s="60">
         <v>2471384</v>
       </c>
       <c r="D45" s="58" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E45" s="60">
         <v>2471384</v>
@@ -2375,33 +2371,33 @@
     </row>
     <row r="46" spans="1:5" ht="15">
       <c r="A46" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="B46" s="56" t="s">
         <v>76</v>
       </c>
-      <c r="B46" s="56" t="s">
-        <v>77</v>
-      </c>
       <c r="C46" s="58" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D46" s="58" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E46" s="58" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="15">
       <c r="A47" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="B47" s="56" t="s">
         <v>78</v>
-      </c>
-      <c r="B47" s="56" t="s">
-        <v>79</v>
       </c>
       <c r="C47" s="61">
         <v>2471384</v>
       </c>
       <c r="D47" s="62" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E47" s="61">
         <v>2471384</v>
@@ -2417,7 +2413,7 @@
     <row r="49" spans="1:5" ht="15">
       <c r="A49" s="20"/>
       <c r="B49" s="56" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C49" s="56"/>
       <c r="D49" s="56"/>
@@ -2425,10 +2421,10 @@
     </row>
     <row r="50" spans="1:5" ht="15">
       <c r="A50" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="B50" s="56" t="s">
         <v>81</v>
-      </c>
-      <c r="B50" s="56" t="s">
-        <v>82</v>
       </c>
       <c r="C50" s="60">
         <v>29116205</v>
@@ -2442,16 +2438,16 @@
     </row>
     <row r="51" spans="1:5" ht="15">
       <c r="A51" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="B51" s="56" t="s">
         <v>83</v>
-      </c>
-      <c r="B51" s="56" t="s">
-        <v>84</v>
       </c>
       <c r="C51" s="60">
         <v>9890048</v>
       </c>
       <c r="D51" s="58" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E51" s="60">
         <v>9890048</v>
@@ -2459,10 +2455,10 @@
     </row>
     <row r="52" spans="1:5" ht="15">
       <c r="A52" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="B52" s="56" t="s">
         <v>85</v>
-      </c>
-      <c r="B52" s="56" t="s">
-        <v>86</v>
       </c>
       <c r="C52" s="60">
         <v>5873482</v>
@@ -2476,10 +2472,10 @@
     </row>
     <row r="53" spans="1:5" ht="15">
       <c r="A53" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="B53" s="56" t="s">
         <v>87</v>
-      </c>
-      <c r="B53" s="56" t="s">
-        <v>88</v>
       </c>
       <c r="C53" s="65">
         <v>44879735</v>
@@ -2501,13 +2497,13 @@
     <row r="55" spans="1:5" ht="15">
       <c r="A55" s="17"/>
       <c r="B55" s="67" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C55" s="67"/>
       <c r="D55" s="67"/>
       <c r="E55" s="67"/>
     </row>
-    <row r="56" spans="1:5" ht="15.75">
+    <row r="56" spans="1:5" ht="16">
       <c r="C56" s="66"/>
     </row>
   </sheetData>
@@ -2523,24 +2519,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="59.42578125" style="25" customWidth="1"/>
-    <col min="2" max="2" width="38.140625" style="25" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" style="25" customWidth="1"/>
-    <col min="4" max="4" width="55.7109375" style="25" customWidth="1"/>
-    <col min="5" max="5" width="23.7109375" style="25" customWidth="1"/>
-    <col min="6" max="6" width="19.85546875" style="25" customWidth="1"/>
-    <col min="7" max="7" width="24.5703125" style="25" customWidth="1"/>
-    <col min="8" max="8" width="55.7109375" style="25" customWidth="1"/>
-    <col min="9" max="9" width="22.140625" style="25" customWidth="1"/>
-    <col min="10" max="10" width="21.85546875" style="25" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" style="25" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="25"/>
+    <col min="1" max="1" width="59.5" style="25" customWidth="1"/>
+    <col min="2" max="2" width="38.1640625" style="25" customWidth="1"/>
+    <col min="3" max="3" width="22.1640625" style="25" customWidth="1"/>
+    <col min="4" max="4" width="55.6640625" style="25" customWidth="1"/>
+    <col min="5" max="5" width="23.6640625" style="25" customWidth="1"/>
+    <col min="6" max="6" width="19.83203125" style="25" customWidth="1"/>
+    <col min="7" max="7" width="24.5" style="25" customWidth="1"/>
+    <col min="8" max="8" width="55.6640625" style="25" customWidth="1"/>
+    <col min="9" max="9" width="22.1640625" style="25" customWidth="1"/>
+    <col min="10" max="10" width="21.83203125" style="25" customWidth="1"/>
+    <col min="11" max="11" width="9.1640625" style="25" customWidth="1"/>
+    <col min="12" max="16384" width="9.1640625" style="25"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15">
@@ -2562,7 +2558,7 @@
     <row r="3" spans="1:11" ht="15">
       <c r="A3" s="2"/>
       <c r="B3" s="26" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D3" s="14"/>
       <c r="H3" s="14"/>
@@ -2570,7 +2566,7 @@
     <row r="4" spans="1:11" ht="15">
       <c r="A4" s="2"/>
       <c r="B4" s="27" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C4" s="28"/>
       <c r="D4" s="29"/>
@@ -2581,7 +2577,7 @@
       <c r="I4" s="28"/>
       <c r="J4" s="28"/>
     </row>
-    <row r="5" spans="1:11" ht="23.25">
+    <row r="5" spans="1:11" ht="15">
       <c r="A5" s="2"/>
       <c r="B5" s="30"/>
       <c r="D5" s="31"/>
@@ -2590,13 +2586,13 @@
       <c r="G5" s="33"/>
       <c r="H5" s="31"/>
       <c r="I5" s="44" t="s">
+        <v>91</v>
+      </c>
+      <c r="J5" s="44" t="s">
         <v>92</v>
       </c>
-      <c r="J5" s="44" t="s">
+      <c r="K5" s="44" t="s">
         <v>93</v>
-      </c>
-      <c r="K5" s="44" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="15">
@@ -2611,27 +2607,27 @@
       <c r="J6" s="36"/>
       <c r="K6" s="34"/>
     </row>
-    <row r="7" spans="1:11" ht="27">
+    <row r="7" spans="1:11" ht="28">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="37" t="s">
+        <v>94</v>
+      </c>
+      <c r="C7" s="38" t="s">
         <v>95</v>
-      </c>
-      <c r="C7" s="38" t="s">
-        <v>96</v>
       </c>
       <c r="D7" s="39" t="s">
         <v>4</v>
       </c>
       <c r="E7" s="40" t="s">
+        <v>96</v>
+      </c>
+      <c r="F7" s="40" t="s">
         <v>97</v>
       </c>
-      <c r="F7" s="40" t="s">
+      <c r="G7" s="40" t="s">
         <v>98</v>
-      </c>
-      <c r="G7" s="40" t="s">
-        <v>99</v>
       </c>
       <c r="H7" s="39" t="s">
         <v>4</v>
@@ -2640,35 +2636,35 @@
         <v>5</v>
       </c>
       <c r="J7" s="40" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K7" s="40" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="15">
       <c r="A8" s="2"/>
       <c r="B8" s="41" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D8" s="14"/>
       <c r="H8" s="14"/>
     </row>
-    <row r="9" spans="1:11" ht="23.25">
+    <row r="9" spans="1:11" ht="25">
       <c r="A9" s="2"/>
-      <c r="B9" s="70"/>
+      <c r="B9" s="42"/>
       <c r="C9" s="44" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="44" t="s">
+        <v>101</v>
+      </c>
+      <c r="F9" s="44" t="s">
         <v>102</v>
       </c>
-      <c r="F9" s="44" t="s">
+      <c r="G9" s="44" t="s">
         <v>103</v>
-      </c>
-      <c r="G9" s="44" t="s">
-        <v>104</v>
       </c>
       <c r="H9" s="14"/>
     </row>
@@ -2682,16 +2678,16 @@
     </row>
     <row r="11" spans="1:11" ht="15">
       <c r="A11" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B11" s="42" t="s">
         <v>105</v>
-      </c>
-      <c r="B11" s="42" t="s">
-        <v>106</v>
       </c>
       <c r="C11" s="45">
         <v>2629048</v>
       </c>
       <c r="D11" s="46" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E11" s="45">
         <v>437626</v>
@@ -2700,16 +2696,16 @@
         <v>13808</v>
       </c>
       <c r="G11" s="36" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H11" s="46" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I11" s="45">
         <v>-2177614</v>
       </c>
       <c r="J11" s="36" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K11" s="45">
         <v>-2177614</v>
@@ -2717,10 +2713,10 @@
     </row>
     <row r="12" spans="1:11" ht="15">
       <c r="A12" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B12" s="42" t="s">
         <v>109</v>
-      </c>
-      <c r="B12" s="42" t="s">
-        <v>110</v>
       </c>
       <c r="C12" s="47">
         <v>2736817</v>
@@ -2736,16 +2732,16 @@
         <v>397461</v>
       </c>
       <c r="G12" s="36" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H12" s="46" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I12" s="47">
         <v>-2291064</v>
       </c>
       <c r="J12" s="36" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K12" s="47">
         <v>-2291064</v>
@@ -2753,16 +2749,16 @@
     </row>
     <row r="13" spans="1:11" ht="15">
       <c r="A13" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B13" s="42" t="s">
         <v>112</v>
-      </c>
-      <c r="B13" s="42" t="s">
-        <v>113</v>
       </c>
       <c r="C13" s="47">
         <v>2509096</v>
       </c>
       <c r="D13" s="46" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E13" s="47">
         <v>331218</v>
@@ -2774,13 +2770,13 @@
         <v>44634</v>
       </c>
       <c r="H13" s="46" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I13" s="47">
         <v>210869</v>
       </c>
       <c r="J13" s="36" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K13" s="47">
         <v>210869</v>
@@ -2788,10 +2784,10 @@
     </row>
     <row r="14" spans="1:11" ht="15">
       <c r="A14" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B14" s="42" t="s">
         <v>116</v>
-      </c>
-      <c r="B14" s="42" t="s">
-        <v>117</v>
       </c>
       <c r="C14" s="47">
         <v>356450</v>
@@ -2804,19 +2800,19 @@
         <v>142299</v>
       </c>
       <c r="F14" s="36" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G14" s="47">
         <v>76140</v>
       </c>
       <c r="H14" s="46" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I14" s="47">
         <v>-138011</v>
       </c>
       <c r="J14" s="36" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K14" s="47">
         <v>-138011</v>
@@ -2824,10 +2820,10 @@
     </row>
     <row r="15" spans="1:11" ht="15">
       <c r="A15" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B15" s="42" t="s">
         <v>119</v>
-      </c>
-      <c r="B15" s="42" t="s">
-        <v>120</v>
       </c>
       <c r="C15" s="47">
         <v>729729</v>
@@ -2840,19 +2836,19 @@
         <v>42903</v>
       </c>
       <c r="F15" s="36" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G15" s="36" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H15" s="46" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I15" s="47">
         <v>-686826</v>
       </c>
       <c r="J15" s="36" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K15" s="47">
         <v>-686826</v>
@@ -2860,16 +2856,16 @@
     </row>
     <row r="16" spans="1:11" ht="15">
       <c r="A16" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B16" s="42" t="s">
         <v>122</v>
-      </c>
-      <c r="B16" s="42" t="s">
-        <v>123</v>
       </c>
       <c r="C16" s="47">
         <v>8961140</v>
       </c>
       <c r="D16" s="46" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E16" s="47">
         <v>1002338</v>
@@ -2881,13 +2877,13 @@
         <v>120774</v>
       </c>
       <c r="H16" s="46" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I16" s="47">
         <v>-5082646</v>
       </c>
       <c r="J16" s="36" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K16" s="47">
         <v>-5082646</v>
@@ -2896,7 +2892,7 @@
     <row r="17" spans="1:11" ht="15">
       <c r="A17" s="2"/>
       <c r="B17" s="42" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C17" s="34"/>
       <c r="D17" s="46" t="str">
@@ -2907,27 +2903,27 @@
       <c r="F17" s="34"/>
       <c r="G17" s="34"/>
       <c r="H17" s="46" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I17" s="34"/>
       <c r="J17" s="34"/>
       <c r="K17" s="34"/>
     </row>
-    <row r="18" spans="1:11" ht="42.95" customHeight="1">
+    <row r="18" spans="1:11" ht="43" customHeight="1">
       <c r="A18" s="2"/>
       <c r="B18" s="42"/>
       <c r="C18" s="44" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D18" s="46"/>
       <c r="E18" s="44" t="s">
+        <v>128</v>
+      </c>
+      <c r="F18" s="44" t="s">
         <v>129</v>
       </c>
-      <c r="F18" s="44" t="s">
+      <c r="G18" s="44" t="s">
         <v>130</v>
-      </c>
-      <c r="G18" s="44" t="s">
-        <v>131</v>
       </c>
       <c r="H18" s="46"/>
       <c r="I18" s="34"/>
@@ -2936,31 +2932,31 @@
     </row>
     <row r="19" spans="1:11" ht="15">
       <c r="A19" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B19" s="42" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C19" s="47">
         <v>60694</v>
       </c>
       <c r="D19" s="46" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E19" s="47">
         <v>16847</v>
       </c>
       <c r="F19" s="36" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G19" s="36" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H19" s="46" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I19" s="36" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J19" s="47">
         <v>-43847</v>
@@ -2969,54 +2965,54 @@
         <v>-43847</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="23.25">
+    <row r="20" spans="1:11" ht="25">
       <c r="A20" s="2"/>
       <c r="B20" s="42"/>
       <c r="C20" s="44" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D20" s="46"/>
       <c r="E20" s="44" t="s">
+        <v>132</v>
+      </c>
+      <c r="F20" s="44" t="s">
         <v>133</v>
       </c>
-      <c r="F20" s="44" t="s">
+      <c r="G20" s="44" t="s">
         <v>134</v>
-      </c>
-      <c r="G20" s="44" t="s">
-        <v>135</v>
       </c>
       <c r="H20" s="46"/>
       <c r="I20" s="36"/>
       <c r="J20" s="47"/>
       <c r="K20" s="47"/>
     </row>
-    <row r="21" spans="1:11" ht="15.75">
+    <row r="21" spans="1:11" ht="15">
       <c r="A21" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B21" s="48" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C21" s="47">
         <v>60694</v>
       </c>
       <c r="D21" s="46" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E21" s="47">
         <v>16847</v>
       </c>
       <c r="F21" s="36" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G21" s="36" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H21" s="46" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I21" s="36" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J21" s="47">
         <v>-43847</v>
@@ -3025,21 +3021,21 @@
         <v>-43847</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="24">
+    <row r="22" spans="1:11" ht="15">
       <c r="A22" s="2"/>
       <c r="B22" s="48"/>
       <c r="C22" s="43" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D22" s="46"/>
       <c r="E22" s="44" t="s">
+        <v>136</v>
+      </c>
+      <c r="F22" s="44" t="s">
         <v>137</v>
       </c>
-      <c r="F22" s="44" t="s">
+      <c r="G22" s="44" t="s">
         <v>138</v>
-      </c>
-      <c r="G22" s="44" t="s">
-        <v>139</v>
       </c>
       <c r="H22" s="46"/>
       <c r="I22" s="36"/>
@@ -3048,16 +3044,16 @@
     </row>
     <row r="23" spans="1:11" ht="15">
       <c r="A23" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B23" s="42" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C23" s="45">
         <v>9021834</v>
       </c>
       <c r="D23" s="46" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E23" s="45">
         <v>1019185</v>
@@ -3069,7 +3065,7 @@
         <v>120774</v>
       </c>
       <c r="H23" s="46" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I23" s="47">
         <v>-5082646</v>
@@ -3094,11 +3090,11 @@
       <c r="J24" s="47"/>
       <c r="K24" s="47"/>
     </row>
-    <row r="25" spans="1:11" ht="15.75">
+    <row r="25" spans="1:11" ht="15">
       <c r="A25" s="2"/>
       <c r="D25" s="50"/>
       <c r="E25" s="68" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F25" s="68"/>
       <c r="G25" s="34"/>
@@ -3108,7 +3104,7 @@
       <c r="A26" s="2"/>
       <c r="D26" s="50"/>
       <c r="E26" s="69" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F26" s="69"/>
       <c r="G26" s="34"/>
@@ -3121,18 +3117,18 @@
       <c r="A27" s="2"/>
       <c r="D27" s="51"/>
       <c r="E27" s="69" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F27" s="69"/>
       <c r="G27" s="34"/>
       <c r="H27" s="51" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I27" s="47">
         <v>2846766</v>
       </c>
       <c r="J27" s="36" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K27" s="47">
         <v>2846766</v>
@@ -3142,18 +3138,18 @@
       <c r="A28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="69" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F28" s="69"/>
       <c r="G28" s="34"/>
       <c r="H28" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="I28" s="47">
         <v>1348657</v>
       </c>
       <c r="J28" s="36" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K28" s="47">
         <v>1348657</v>
@@ -3163,18 +3159,18 @@
       <c r="A29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="69" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F29" s="69"/>
       <c r="G29" s="34"/>
       <c r="H29" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I29" s="47">
         <v>563908</v>
       </c>
       <c r="J29" s="36" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K29" s="47">
         <v>563908</v>
@@ -3184,28 +3180,28 @@
       <c r="A30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="69" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F30" s="69"/>
       <c r="G30" s="34"/>
       <c r="H30" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I30" s="47">
         <v>162881</v>
       </c>
       <c r="J30" s="36" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K30" s="47">
         <v>162881</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="15.75">
+    <row r="31" spans="1:11" ht="15">
       <c r="A31" s="2"/>
       <c r="D31" s="2"/>
       <c r="E31" s="68" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F31" s="68"/>
       <c r="G31" s="34"/>
@@ -3214,7 +3210,7 @@
         <v>4922212</v>
       </c>
       <c r="J31" s="36" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K31" s="47">
         <v>4922212</v>
@@ -3224,18 +3220,18 @@
       <c r="A32" s="2"/>
       <c r="D32" s="2"/>
       <c r="E32" s="69" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F32" s="69"/>
       <c r="G32" s="34"/>
       <c r="H32" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="I32" s="47">
         <v>587740</v>
       </c>
       <c r="J32" s="36" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K32" s="47">
         <v>587740</v>
@@ -3245,18 +3241,18 @@
       <c r="A33" s="2"/>
       <c r="D33" s="2"/>
       <c r="E33" s="69" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F33" s="69"/>
       <c r="G33" s="34"/>
       <c r="H33" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I33" s="47">
         <v>174443</v>
       </c>
       <c r="J33" s="36" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K33" s="47">
         <v>174443</v>
@@ -3266,18 +3262,18 @@
       <c r="A34" s="2"/>
       <c r="D34" s="51"/>
       <c r="E34" s="69" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F34" s="69"/>
       <c r="G34" s="34"/>
       <c r="H34" s="51" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I34" s="47">
         <v>-281502</v>
       </c>
       <c r="J34" s="36" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K34" s="47">
         <v>-281502</v>
@@ -3287,18 +3283,18 @@
       <c r="A35" s="2"/>
       <c r="D35" s="51"/>
       <c r="E35" s="69" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F35" s="69"/>
       <c r="G35" s="34"/>
       <c r="H35" s="51" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I35" s="47">
         <v>54512</v>
       </c>
       <c r="J35" s="36" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K35" s="47">
         <v>54512</v>
@@ -3308,54 +3304,54 @@
       <c r="A36" s="2"/>
       <c r="D36" s="2"/>
       <c r="E36" s="69" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F36" s="69"/>
       <c r="G36" s="34"/>
       <c r="H36" s="51" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="I36" s="47">
         <v>6958</v>
       </c>
       <c r="J36" s="36" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K36" s="47">
         <v>6958</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="15.75">
+    <row r="37" spans="1:11" ht="15">
       <c r="A37" s="2"/>
       <c r="D37" s="51"/>
       <c r="E37" s="68" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F37" s="68"/>
       <c r="G37" s="34"/>
       <c r="H37" s="51" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I37" s="47">
         <v>5464363</v>
       </c>
       <c r="J37" s="36" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K37" s="47">
         <v>5464363</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="15.75">
+    <row r="38" spans="1:11" ht="15">
       <c r="A38" s="2"/>
       <c r="D38" s="51"/>
       <c r="E38" s="68" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F38" s="68"/>
       <c r="G38" s="34"/>
       <c r="H38" s="51" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I38" s="47">
         <v>381717</v>
@@ -3367,16 +3363,16 @@
         <v>337870</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="15.75">
+    <row r="39" spans="1:11" ht="15">
       <c r="A39" s="2"/>
       <c r="D39" s="51"/>
       <c r="E39" s="68" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F39" s="68"/>
       <c r="G39" s="34"/>
       <c r="H39" s="51" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I39" s="47">
         <v>44498018</v>
@@ -3388,16 +3384,16 @@
         <v>45422004</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="15.75">
+    <row r="40" spans="1:11" ht="15">
       <c r="A40" s="2"/>
       <c r="D40" s="51"/>
       <c r="E40" s="68" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F40" s="68"/>
       <c r="G40" s="34"/>
       <c r="H40" s="51" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I40" s="45">
         <v>44879735</v>
@@ -3409,7 +3405,7 @@
         <v>45759874</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="15.75">
+    <row r="41" spans="1:11" ht="15">
       <c r="A41" s="2"/>
       <c r="D41" s="14"/>
       <c r="E41" s="68"/>
@@ -3422,23 +3418,13 @@
     <row r="42" spans="1:11" ht="15">
       <c r="A42" s="2"/>
       <c r="B42" s="52" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D42" s="14"/>
       <c r="H42" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
     <mergeCell ref="E40:F40"/>
     <mergeCell ref="E41:F41"/>
     <mergeCell ref="E35:F35"/>
@@ -3446,6 +3432,16 @@
     <mergeCell ref="E37:F37"/>
     <mergeCell ref="E38:F38"/>
     <mergeCell ref="E39:F39"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -3460,17 +3456,17 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="82" style="16" customWidth="1"/>
-    <col min="2" max="2" width="38.85546875" style="16" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" style="16" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" style="16" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" style="16" customWidth="1"/>
-    <col min="6" max="7" width="13.42578125" style="16" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" style="16" customWidth="1"/>
-    <col min="9" max="9" width="11.140625" style="16" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="16"/>
+    <col min="2" max="2" width="38.83203125" style="16" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" style="16" customWidth="1"/>
+    <col min="4" max="4" width="13.5" style="16" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" style="16" customWidth="1"/>
+    <col min="6" max="7" width="13.5" style="16" customWidth="1"/>
+    <col min="8" max="8" width="12.5" style="16" customWidth="1"/>
+    <col min="9" max="9" width="11.1640625" style="16" customWidth="1"/>
+    <col min="10" max="16384" width="9.1640625" style="16"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15">
@@ -3483,21 +3479,21 @@
     <row r="2" spans="1:9" ht="15">
       <c r="A2" s="17"/>
       <c r="B2" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:9" ht="15">
       <c r="A3" s="17"/>
       <c r="B3" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:9" ht="15">
       <c r="A4" s="17"/>
       <c r="B4" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F4" s="1"/>
     </row>
@@ -3506,47 +3502,47 @@
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="19" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E5" s="19"/>
       <c r="F5" s="19"/>
       <c r="G5" s="19" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9" ht="45">
+    <row r="6" spans="1:9" ht="48">
       <c r="A6" s="20" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="E6" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="F6" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="G6" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="H6" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="H6" s="4" t="s">
-        <v>177</v>
-      </c>
       <c r="I6" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="15">
       <c r="A7" s="17"/>
       <c r="B7" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -3558,28 +3554,28 @@
     </row>
     <row r="8" spans="1:9" ht="15">
       <c r="A8" s="20" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C8" s="7">
         <v>2846766</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I8" s="7">
         <v>2846766</v>
@@ -3587,28 +3583,28 @@
     </row>
     <row r="9" spans="1:9" ht="15">
       <c r="A9" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>181</v>
-      </c>
       <c r="C9" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E9" s="8">
         <v>111400</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I9" s="8">
         <v>111400</v>
@@ -3616,25 +3612,25 @@
     </row>
     <row r="10" spans="1:9" ht="15">
       <c r="A10" s="20" t="s">
+        <v>181</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>183</v>
-      </c>
       <c r="C10" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D10" s="8">
         <v>1204882</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H10" s="8">
         <v>442230</v>
@@ -3645,28 +3641,28 @@
     </row>
     <row r="11" spans="1:9" ht="15">
       <c r="A11" s="20" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C11" s="8">
         <v>563908</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I11" s="8">
         <v>563908</v>
@@ -3674,28 +3670,28 @@
     </row>
     <row r="12" spans="1:9" ht="15">
       <c r="A12" s="20" t="s">
+        <v>184</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>185</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>186</v>
       </c>
       <c r="C12" s="8">
         <v>162881</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I12" s="8">
         <v>162881</v>
@@ -3703,25 +3699,25 @@
     </row>
     <row r="13" spans="1:9" ht="15">
       <c r="A13" s="20" t="s">
+        <v>186</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>187</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="C13" s="8">
         <v>114026</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H13" s="8">
         <v>140326</v>
@@ -3732,28 +3728,28 @@
     </row>
     <row r="14" spans="1:9" ht="15">
       <c r="A14" s="20" t="s">
+        <v>188</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>189</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>190</v>
       </c>
       <c r="C14" s="8">
         <v>151409</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I14" s="8">
         <v>151409</v>
@@ -3761,25 +3757,25 @@
     </row>
     <row r="15" spans="1:9" ht="15">
       <c r="A15" s="20" t="s">
+        <v>190</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>191</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>192</v>
       </c>
       <c r="C15" s="8">
         <v>135233</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F15" s="8">
         <v>1467024</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H15" s="8">
         <v>1170041</v>
@@ -3790,19 +3786,19 @@
     </row>
     <row r="16" spans="1:9" ht="15">
       <c r="A16" s="20" t="s">
+        <v>192</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>194</v>
-      </c>
       <c r="C16" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
@@ -3811,28 +3807,28 @@
     </row>
     <row r="17" spans="1:9" ht="15">
       <c r="A17" s="20" t="s">
+        <v>194</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>195</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>196</v>
       </c>
       <c r="C17" s="8">
         <v>174443</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I17" s="8">
         <v>174443</v>
@@ -3840,28 +3836,28 @@
     </row>
     <row r="18" spans="1:9" ht="15">
       <c r="A18" s="20" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C18" s="8">
         <v>587740</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I18" s="8">
         <v>587740</v>
@@ -3869,28 +3865,28 @@
     </row>
     <row r="19" spans="1:9" ht="15">
       <c r="A19" s="20" t="s">
+        <v>197</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>198</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>199</v>
       </c>
       <c r="C19" s="8">
         <v>305645</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I19" s="8">
         <v>305645</v>
@@ -3898,10 +3894,10 @@
     </row>
     <row r="20" spans="1:9" ht="15">
       <c r="A20" s="20" t="s">
+        <v>199</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>200</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>201</v>
       </c>
       <c r="C20" s="8">
         <v>-185018</v>
@@ -3913,7 +3909,7 @@
         <v>17961</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G20" s="8">
         <v>-80986</v>
@@ -3927,25 +3923,25 @@
     </row>
     <row r="21" spans="1:9" ht="15">
       <c r="A21" s="20" t="s">
+        <v>201</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>202</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>203</v>
       </c>
       <c r="C21" s="8">
         <v>40844</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H21" s="11">
         <v>648</v>
@@ -3956,10 +3952,10 @@
     </row>
     <row r="22" spans="1:9" ht="15">
       <c r="A22" s="20" t="s">
+        <v>203</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>204</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>205</v>
       </c>
       <c r="C22" s="8">
         <v>4897877</v>
@@ -3997,7 +3993,7 @@
     <row r="24" spans="1:9" ht="15">
       <c r="A24" s="20"/>
       <c r="B24" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
@@ -4010,7 +4006,7 @@
     <row r="25" spans="1:9" ht="15">
       <c r="A25" s="20"/>
       <c r="B25" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
@@ -4022,25 +4018,25 @@
     </row>
     <row r="26" spans="1:9" ht="15">
       <c r="A26" s="20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C26" s="8">
         <v>2570417</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H26" s="8">
         <v>126650</v>
@@ -4051,25 +4047,25 @@
     </row>
     <row r="27" spans="1:9" ht="15">
       <c r="A27" s="20" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C27" s="8">
         <v>2684319</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H27" s="8">
         <v>130541</v>
@@ -4080,10 +4076,10 @@
     </row>
     <row r="28" spans="1:9" ht="15">
       <c r="A28" s="20" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C28" s="8">
         <v>333423</v>
@@ -4092,13 +4088,13 @@
         <v>1424676</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H28" s="8">
         <v>383356</v>
@@ -4109,28 +4105,28 @@
     </row>
     <row r="29" spans="1:9" ht="15">
       <c r="A29" s="20" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C29" s="8">
         <v>299175</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H29" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I29" s="8">
         <v>299175</v>
@@ -4138,25 +4134,25 @@
     </row>
     <row r="30" spans="1:9" ht="15">
       <c r="A30" s="20" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C30" s="8">
         <v>336592</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H30" s="8">
         <v>140808</v>
@@ -4167,10 +4163,10 @@
     </row>
     <row r="31" spans="1:9" ht="15">
       <c r="A31" s="20" t="s">
+        <v>212</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>213</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>214</v>
       </c>
       <c r="C31" s="8">
         <v>22168</v>
@@ -4179,10 +4175,10 @@
         <v>161367</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G31" s="8">
         <v>869925</v>
@@ -4196,10 +4192,10 @@
     </row>
     <row r="32" spans="1:9" ht="15">
       <c r="A32" s="20" t="s">
+        <v>214</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>215</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>216</v>
       </c>
       <c r="C32" s="8">
         <v>6246094</v>
@@ -4208,10 +4204,10 @@
         <v>1586043</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G32" s="8">
         <v>869925</v>
@@ -4225,10 +4221,10 @@
     </row>
     <row r="33" spans="1:9" ht="32.25" customHeight="1">
       <c r="A33" s="20" t="s">
+        <v>216</v>
+      </c>
+      <c r="B33" s="5" t="s">
         <v>217</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>218</v>
       </c>
       <c r="C33" s="8">
         <v>-1348217</v>
@@ -4255,7 +4251,7 @@
     <row r="34" spans="1:9" ht="15">
       <c r="A34" s="20"/>
       <c r="B34" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C34" s="6"/>
       <c r="D34" s="6"/>
@@ -4267,28 +4263,28 @@
     </row>
     <row r="35" spans="1:9" ht="15">
       <c r="A35" s="20" t="s">
+        <v>219</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="B35" s="1" t="s">
-        <v>221</v>
-      </c>
       <c r="C35" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E35" s="8">
         <v>58091</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H35" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I35" s="8">
         <v>58091</v>
@@ -4296,22 +4292,22 @@
     </row>
     <row r="36" spans="1:9" ht="15">
       <c r="A36" s="20" t="s">
+        <v>221</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>222</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>223</v>
       </c>
       <c r="C36" s="8">
         <v>1597681</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F36" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G36" s="8">
         <v>1632609</v>
@@ -4325,25 +4321,25 @@
     </row>
     <row r="37" spans="1:9" ht="15">
       <c r="A37" s="20" t="s">
+        <v>223</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="B37" s="1" t="s">
-        <v>225</v>
-      </c>
       <c r="C37" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D37" s="8">
         <v>-41809</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F37" s="8">
         <v>-1467024</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H37" s="8">
         <v>-1742671</v>
@@ -4354,10 +4350,10 @@
     </row>
     <row r="38" spans="1:9" ht="15">
       <c r="A38" s="20" t="s">
+        <v>225</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>226</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>227</v>
       </c>
       <c r="C38" s="8">
         <v>1597681</v>
@@ -4383,10 +4379,10 @@
     </row>
     <row r="39" spans="1:9" ht="15">
       <c r="A39" s="20" t="s">
+        <v>227</v>
+      </c>
+      <c r="B39" s="1" t="s">
         <v>228</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>229</v>
       </c>
       <c r="C39" s="8">
         <v>249464</v>
@@ -4405,13 +4401,13 @@
     <row r="40" spans="1:9" ht="15">
       <c r="A40" s="20"/>
       <c r="B40" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C40" s="6"/>
       <c r="D40" s="6"/>
       <c r="E40" s="6"/>
       <c r="F40" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G40" s="8">
         <v>681698</v>
@@ -4425,10 +4421,10 @@
     </row>
     <row r="41" spans="1:9" ht="15">
       <c r="A41" s="20" t="s">
+        <v>230</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>231</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>232</v>
       </c>
       <c r="C41" s="8">
         <v>6163893</v>
@@ -4440,7 +4436,7 @@
         <v>5430243</v>
       </c>
       <c r="F41" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G41" s="8">
         <v>1924746</v>
@@ -4454,10 +4450,10 @@
     </row>
     <row r="42" spans="1:9" ht="15">
       <c r="A42" s="20" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C42" s="7">
         <v>6413357</v>
@@ -4469,7 +4465,7 @@
         <v>5617695</v>
       </c>
       <c r="F42" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G42" s="7">
         <v>2606444</v>
@@ -4491,10 +4487,10 @@
     </row>
     <row r="44" spans="1:9" ht="15">
       <c r="B44" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" ht="15.75">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="16">
       <c r="C45" s="24"/>
     </row>
   </sheetData>
@@ -4510,18 +4506,18 @@
       <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="75.28515625" style="16" customWidth="1"/>
+    <col min="1" max="1" width="75.33203125" style="16" customWidth="1"/>
     <col min="2" max="2" width="38" style="16" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" style="16" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" style="16" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" style="16" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" style="16" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" style="16" customWidth="1"/>
-    <col min="8" max="8" width="14.85546875" style="16" customWidth="1"/>
-    <col min="9" max="9" width="12.85546875" style="16" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="16"/>
+    <col min="3" max="3" width="14.33203125" style="16" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" style="16" customWidth="1"/>
+    <col min="5" max="5" width="15.83203125" style="16" customWidth="1"/>
+    <col min="6" max="6" width="16.5" style="16" customWidth="1"/>
+    <col min="7" max="7" width="15.5" style="16" customWidth="1"/>
+    <col min="8" max="8" width="14.83203125" style="16" customWidth="1"/>
+    <col min="9" max="9" width="12.83203125" style="16" customWidth="1"/>
+    <col min="10" max="16384" width="9.1640625" style="16"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15">
@@ -4533,14 +4529,14 @@
     <row r="2" spans="1:9" ht="15">
       <c r="A2" s="17"/>
       <c r="B2" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:9" ht="15">
       <c r="A3" s="17"/>
       <c r="B3" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F3" s="1"/>
     </row>
@@ -4555,51 +4551,51 @@
       <c r="A5" s="17"/>
       <c r="D5" s="18"/>
       <c r="E5" s="19" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F5" s="19"/>
       <c r="G5" s="19" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="45">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="48">
       <c r="A6" s="20" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="E6" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="F6" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="G6" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="H6" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="H6" s="4" t="s">
-        <v>177</v>
-      </c>
       <c r="I6" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="15">
       <c r="A7" s="17"/>
       <c r="B7" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="15">
       <c r="A8" s="20" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8" s="7">
         <v>5985880</v>
@@ -4611,7 +4607,7 @@
         <v>1857892</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G8" s="7">
         <v>2674360</v>
@@ -4625,23 +4621,23 @@
     </row>
     <row r="9" spans="1:9" ht="15">
       <c r="A9" s="20" t="s">
+        <v>235</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>236</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>237</v>
       </c>
       <c r="C9" s="8">
         <v>646294</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F9" s="21"/>
       <c r="G9" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H9" s="8">
         <v>487021</v>
@@ -4652,26 +4648,26 @@
     </row>
     <row r="10" spans="1:9" ht="15">
       <c r="A10" s="20" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C10" s="8">
         <v>25257</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F10" s="21"/>
       <c r="G10" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I10" s="8">
         <v>25257</v>
@@ -4679,26 +4675,26 @@
     </row>
     <row r="11" spans="1:9" ht="15">
       <c r="A11" s="20" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E11" s="8">
         <v>3170453</v>
       </c>
       <c r="F11" s="21"/>
       <c r="G11" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I11" s="8">
         <v>3170453</v>
@@ -4706,26 +4702,26 @@
     </row>
     <row r="12" spans="1:9" ht="15">
       <c r="A12" s="20" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E12" s="8">
         <v>3311550</v>
       </c>
       <c r="F12" s="21"/>
       <c r="G12" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I12" s="8">
         <v>3311550</v>
@@ -4733,26 +4729,26 @@
     </row>
     <row r="13" spans="1:9" ht="15">
       <c r="A13" s="20" t="s">
+        <v>240</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>241</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>242</v>
       </c>
       <c r="C13" s="8">
         <v>52578</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F13" s="21"/>
       <c r="G13" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I13" s="8">
         <v>52578</v>
@@ -4760,26 +4756,26 @@
     </row>
     <row r="14" spans="1:9" ht="15">
       <c r="A14" s="20" t="s">
+        <v>242</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>243</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>244</v>
       </c>
       <c r="C14" s="8">
         <v>120893</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F14" s="21"/>
       <c r="G14" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I14" s="8">
         <v>120893</v>
@@ -4787,22 +4783,22 @@
     </row>
     <row r="15" spans="1:9" ht="15">
       <c r="A15" s="20" t="s">
+        <v>244</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>246</v>
-      </c>
       <c r="C15" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G15" s="21"/>
       <c r="H15" s="21"/>
@@ -4810,10 +4806,10 @@
     </row>
     <row r="16" spans="1:9" ht="15">
       <c r="A16" s="20" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C16" s="7">
         <v>6830902</v>
@@ -4825,7 +4821,7 @@
         <v>8339895</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G16" s="7">
         <v>2674360</v>
@@ -4851,13 +4847,13 @@
     <row r="18" spans="1:9" ht="15">
       <c r="A18" s="20"/>
       <c r="B18" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C18" s="21"/>
       <c r="D18" s="21"/>
       <c r="E18" s="21"/>
       <c r="F18" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G18" s="21"/>
       <c r="H18" s="21"/>
@@ -4866,13 +4862,13 @@
     <row r="19" spans="1:9" ht="15">
       <c r="A19" s="20"/>
       <c r="B19" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C19" s="21"/>
       <c r="D19" s="21"/>
       <c r="E19" s="21"/>
       <c r="F19" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G19" s="21"/>
       <c r="H19" s="21"/>
@@ -4881,13 +4877,13 @@
     <row r="20" spans="1:9" ht="15">
       <c r="A20" s="20"/>
       <c r="B20" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C20" s="21"/>
       <c r="D20" s="21"/>
       <c r="E20" s="21"/>
       <c r="F20" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G20" s="21"/>
       <c r="H20" s="21"/>
@@ -4895,10 +4891,10 @@
     </row>
     <row r="21" spans="1:9" ht="15">
       <c r="A21" s="20" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C21" s="7">
         <v>1826</v>
@@ -4907,10 +4903,10 @@
         <v>54858</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G21" s="7">
         <v>67916</v>
@@ -4924,25 +4920,25 @@
     </row>
     <row r="22" spans="1:9" ht="15">
       <c r="A22" s="20" t="s">
+        <v>251</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>252</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>253</v>
       </c>
       <c r="C22" s="8">
         <v>71658</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H22" s="8">
         <v>2700</v>
@@ -4953,28 +4949,28 @@
     </row>
     <row r="23" spans="1:9" ht="15">
       <c r="A23" s="20" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C23" s="11">
         <v>37</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I23" s="11">
         <v>37</v>
@@ -4982,28 +4978,28 @@
     </row>
     <row r="24" spans="1:9" ht="15">
       <c r="A24" s="20" t="s">
+        <v>254</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>255</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>256</v>
       </c>
       <c r="C24" s="8">
         <v>83645</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I24" s="8">
         <v>83645</v>
@@ -5011,25 +5007,25 @@
     </row>
     <row r="25" spans="1:9" ht="15">
       <c r="A25" s="20" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H25" s="8">
         <v>332166</v>
@@ -5040,10 +5036,10 @@
     </row>
     <row r="26" spans="1:9" ht="15">
       <c r="A26" s="20" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C26" s="8">
         <v>157166</v>
@@ -5052,10 +5048,10 @@
         <v>54858</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G26" s="8">
         <v>67916</v>
@@ -5081,13 +5077,13 @@
     <row r="28" spans="1:9" ht="15">
       <c r="A28" s="20"/>
       <c r="B28" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C28" s="21"/>
       <c r="D28" s="21"/>
       <c r="E28" s="21"/>
       <c r="F28" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G28" s="21"/>
       <c r="H28" s="21"/>
@@ -5095,28 +5091,28 @@
     </row>
     <row r="29" spans="1:9" ht="15">
       <c r="A29" s="20" t="s">
+        <v>259</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>260</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>261</v>
       </c>
       <c r="C29" s="8">
         <v>260379</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E29" s="8">
         <v>2722200</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H29" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I29" s="8">
         <v>2982579</v>
@@ -5124,28 +5120,28 @@
     </row>
     <row r="30" spans="1:9" ht="15">
       <c r="A30" s="20" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C30" s="8">
         <v>260379</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E30" s="8">
         <v>2722200</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H30" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I30" s="8">
         <v>2982579</v>
@@ -5165,13 +5161,13 @@
     <row r="32" spans="1:9" ht="15">
       <c r="A32" s="20"/>
       <c r="B32" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C32" s="21"/>
       <c r="D32" s="21"/>
       <c r="E32" s="21"/>
       <c r="F32" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G32" s="21"/>
       <c r="H32" s="21"/>
@@ -5179,28 +5175,28 @@
     </row>
     <row r="33" spans="1:9" ht="15">
       <c r="A33" s="20" t="s">
+        <v>263</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>264</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>265</v>
       </c>
       <c r="C33" s="8">
         <v>173471</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F33" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H33" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I33" s="8">
         <v>173471</v>
@@ -5208,13 +5204,13 @@
     </row>
     <row r="34" spans="1:9" ht="15">
       <c r="A34" s="20" t="s">
+        <v>265</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="B34" s="1" t="s">
-        <v>267</v>
-      </c>
       <c r="C34" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D34" s="8">
         <v>32509</v>
@@ -5224,7 +5220,7 @@
       </c>
       <c r="F34" s="6"/>
       <c r="G34" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H34" s="8">
         <v>1069391</v>
@@ -5235,23 +5231,23 @@
     </row>
     <row r="35" spans="1:9" ht="15">
       <c r="A35" s="20" t="s">
+        <v>267</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>268</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>269</v>
       </c>
       <c r="C35" s="8">
         <v>495019</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F35" s="21"/>
       <c r="G35" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H35" s="8">
         <v>709802</v>
@@ -5262,19 +5258,19 @@
     </row>
     <row r="36" spans="1:9" ht="15">
       <c r="A36" s="20" t="s">
+        <v>269</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>271</v>
-      </c>
       <c r="C36" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D36" s="8">
         <v>606024</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F36" s="21"/>
       <c r="G36" s="8">
@@ -5289,26 +5285,26 @@
     </row>
     <row r="37" spans="1:9" ht="15">
       <c r="A37" s="20" t="s">
+        <v>271</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>272</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>273</v>
       </c>
       <c r="C37" s="8">
         <v>5744867</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F37" s="21"/>
       <c r="G37" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H37" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I37" s="8">
         <v>5744867</v>
@@ -5316,10 +5312,10 @@
     </row>
     <row r="38" spans="1:9" ht="15">
       <c r="A38" s="20" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C38" s="8">
         <v>6413357</v>
@@ -5341,12 +5337,12 @@
         <v>17172907</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="30">
+    <row r="39" spans="1:9" ht="32">
       <c r="A39" s="20" t="s">
+        <v>274</v>
+      </c>
+      <c r="B39" s="5" t="s">
         <v>275</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>276</v>
       </c>
       <c r="C39" s="7">
         <v>6830902</v>
@@ -5381,7 +5377,7 @@
     <row r="41" spans="1:9" ht="15">
       <c r="A41" s="17"/>
       <c r="B41" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -5398,12 +5394,12 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="44.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="66.140625" style="1" customWidth="1"/>
-    <col min="3" max="4" width="19.7109375" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="44.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="66.1640625" style="1" customWidth="1"/>
+    <col min="3" max="4" width="19.6640625" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -5415,7 +5411,7 @@
     <row r="2" spans="1:4">
       <c r="A2" s="2"/>
       <c r="B2" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -5430,21 +5426,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="45">
+    <row r="5" spans="1:4" ht="32">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>278</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="2"/>
       <c r="B6" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
@@ -5452,20 +5448,20 @@
     <row r="7" spans="1:4">
       <c r="A7" s="2"/>
       <c r="B7" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="C8" s="6" t="s">
         <v>11</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>12</v>
       </c>
       <c r="D8" s="7">
         <v>460441</v>
@@ -5473,34 +5469,34 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>282</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>283</v>
       </c>
       <c r="C10" s="8">
         <v>167738</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C11" s="8">
         <v>841465</v>
@@ -5511,10 +5507,10 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="C12" s="8">
         <v>1009203</v>
@@ -5526,7 +5522,7 @@
     <row r="13" spans="1:4">
       <c r="A13" s="2"/>
       <c r="B13" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
@@ -5534,17 +5530,17 @@
     <row r="14" spans="1:4">
       <c r="A14" s="2"/>
       <c r="B14" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>47</v>
       </c>
       <c r="C15" s="8">
         <v>2671</v>
@@ -5555,52 +5551,52 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>49</v>
       </c>
       <c r="C17" s="8">
         <v>5500</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>286</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>287</v>
       </c>
       <c r="C18" s="8">
         <v>120893</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>72</v>
       </c>
       <c r="C19" s="8">
         <v>129064</v>
@@ -5612,17 +5608,17 @@
     <row r="20" spans="1:4">
       <c r="A20" s="2"/>
       <c r="B20" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>82</v>
       </c>
       <c r="C21" s="8">
         <v>1009203</v>
@@ -5633,10 +5629,10 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>86</v>
       </c>
       <c r="C22" s="8">
         <v>-129064</v>
@@ -5647,10 +5643,10 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>88</v>
       </c>
       <c r="C23" s="7">
         <v>880139</v>
@@ -5665,7 +5661,7 @@
     <row r="25" spans="1:4">
       <c r="A25" s="2"/>
       <c r="B25" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -5681,13 +5677,13 @@
       <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="51.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="44.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="51.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="44.33203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="16" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="4" max="4" width="16.83203125" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -5699,46 +5695,46 @@
     <row r="2" spans="1:4">
       <c r="A2" s="2"/>
       <c r="B2" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2"/>
       <c r="B3" s="3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2"/>
       <c r="B4" s="3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="60">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="48">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>278</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="2"/>
       <c r="B6" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>290</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>291</v>
       </c>
       <c r="C7" s="7">
         <v>16847</v>
@@ -5749,10 +5745,10 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>292</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>293</v>
       </c>
       <c r="C8" s="8">
         <v>16847</v>
@@ -5764,31 +5760,31 @@
     <row r="9" spans="1:4">
       <c r="A9" s="2"/>
       <c r="B9" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>295</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>296</v>
       </c>
       <c r="C10" s="8">
         <v>4833</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C11" s="8">
         <v>26989</v>
@@ -5799,10 +5795,10 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>298</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>299</v>
       </c>
       <c r="C12" s="8">
         <v>28872</v>
@@ -5813,10 +5809,10 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>300</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>301</v>
       </c>
       <c r="C13" s="8">
         <v>60694</v>
@@ -5827,10 +5823,10 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>302</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>303</v>
       </c>
       <c r="C14" s="8">
         <v>-43847</v>
@@ -5842,20 +5838,20 @@
     <row r="15" spans="1:4">
       <c r="A15" s="2"/>
       <c r="B15" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>306</v>
-      </c>
       <c r="C16" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D16" s="8">
         <v>6958</v>
@@ -5863,13 +5859,13 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D17" s="8">
         <v>-14675</v>
@@ -5877,13 +5873,13 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>309</v>
-      </c>
       <c r="C18" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D18" s="8">
         <v>-7717</v>
@@ -5891,10 +5887,10 @@
     </row>
     <row r="19" spans="1:4" s="5" customFormat="1" ht="30" customHeight="1">
       <c r="A19" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="B19" s="5" t="s">
         <v>310</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>311</v>
       </c>
       <c r="C19" s="15">
         <v>-43847</v>
@@ -5905,38 +5901,38 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>313</v>
-      </c>
       <c r="C20" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>314</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>315</v>
-      </c>
       <c r="C21" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C22" s="8">
         <v>-43847</v>
@@ -5948,17 +5944,17 @@
     <row r="23" spans="1:4">
       <c r="A23" s="2"/>
       <c r="B23" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C24" s="8">
         <v>923986</v>
@@ -5969,10 +5965,10 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C25" s="7">
         <v>880139</v>
@@ -5987,7 +5983,7 @@
     <row r="27" spans="1:4">
       <c r="A27" s="2"/>
       <c r="B27" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C27" s="13"/>
     </row>
@@ -6004,15 +6000,15 @@
       <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="56.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="66.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="56.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="66.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5" style="1" customWidth="1"/>
     <col min="4" max="4" width="14" style="1" customWidth="1"/>
-    <col min="5" max="7" width="9.140625" style="1"/>
-    <col min="8" max="8" width="21.42578125" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="1"/>
+    <col min="5" max="7" width="9.1640625" style="1"/>
+    <col min="8" max="8" width="21.5" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -6024,47 +6020,47 @@
     <row r="2" spans="1:5">
       <c r="A2" s="2"/>
       <c r="B2" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="2"/>
       <c r="B3" s="3" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="2"/>
       <c r="B4" s="3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="60">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="64">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>278</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>279</v>
       </c>
       <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="2"/>
       <c r="B6" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>321</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>322</v>
       </c>
       <c r="C7" s="7">
         <v>20847</v>
@@ -6075,10 +6071,10 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>323</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>324</v>
       </c>
       <c r="C8" s="8">
         <v>-24734</v>
@@ -6089,27 +6085,27 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>325</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>326</v>
       </c>
       <c r="C9" s="8">
         <v>-4833</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>328</v>
-      </c>
       <c r="C10" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D10" s="8">
         <v>-4428</v>
@@ -6117,10 +6113,10 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>329</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>330</v>
       </c>
       <c r="C11" s="8">
         <v>-8720</v>
@@ -6132,56 +6128,56 @@
     <row r="12" spans="1:5">
       <c r="A12" s="2"/>
       <c r="B12" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>314</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>315</v>
       </c>
       <c r="C13" s="8">
         <v>8720</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>332</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>333</v>
       </c>
       <c r="C14" s="8">
         <v>8720</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="2"/>
       <c r="B15" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>336</v>
-      </c>
       <c r="C16" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D16" s="8">
         <v>-153184</v>
@@ -6189,13 +6185,13 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>337</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>338</v>
-      </c>
       <c r="C17" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D17" s="8">
         <v>6958</v>
@@ -6203,13 +6199,13 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>339</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>340</v>
-      </c>
       <c r="C18" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D18" s="8">
         <v>-146226</v>
@@ -6218,20 +6214,20 @@
     <row r="19" spans="1:4">
       <c r="A19" s="2"/>
       <c r="B19" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>342</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>343</v>
-      </c>
       <c r="C20" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D20" s="8">
         <v>-14675</v>
@@ -6239,27 +6235,27 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>344</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>345</v>
-      </c>
       <c r="C21" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D21" s="8">
         <v>-14675</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" ht="16">
       <c r="A22" s="9" t="s">
+        <v>345</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>346</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>347</v>
-      </c>
       <c r="C22" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D22" s="8">
         <v>-57430</v>
@@ -6268,20 +6264,20 @@
     <row r="23" spans="1:4">
       <c r="A23" s="2"/>
       <c r="B23" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D24" s="8">
         <v>517871</v>
@@ -6289,13 +6285,13 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D25" s="7">
         <v>460441</v>
@@ -6304,7 +6300,7 @@
     <row r="26" spans="1:4">
       <c r="A26" s="2"/>
       <c r="B26" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
@@ -6312,7 +6308,7 @@
     <row r="27" spans="1:4">
       <c r="A27" s="2"/>
       <c r="B27" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
@@ -6320,17 +6316,17 @@
     <row r="28" spans="1:4">
       <c r="A28" s="2"/>
       <c r="B28" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C28" s="6"/>
       <c r="D28" s="6"/>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" ht="16">
       <c r="A29" s="9" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C29" s="7">
         <v>-43847</v>
@@ -6342,7 +6338,7 @@
     <row r="30" spans="1:4">
       <c r="A30" s="2"/>
       <c r="B30" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C30" s="6"/>
       <c r="D30" s="6"/>
@@ -6350,17 +6346,17 @@
     <row r="31" spans="1:4">
       <c r="A31" s="2"/>
       <c r="B31" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>298</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>299</v>
       </c>
       <c r="C32" s="8">
         <v>28872</v>
@@ -6372,17 +6368,17 @@
     <row r="33" spans="1:4">
       <c r="A33" s="2"/>
       <c r="B33" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C33" s="6"/>
       <c r="D33" s="6"/>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>357</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>358</v>
       </c>
       <c r="C34" s="8">
         <v>2255</v>
@@ -6393,38 +6389,38 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>359</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>360</v>
       </c>
       <c r="C35" s="8">
         <v>4000</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>362</v>
-      </c>
       <c r="C36" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>329</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>330</v>
       </c>
       <c r="C37" s="7">
         <v>-8720</v>
@@ -6439,7 +6435,7 @@
     <row r="39" spans="1:4">
       <c r="A39" s="2"/>
       <c r="B39" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C39" s="13"/>
     </row>

</xml_diff>